<commit_message>
insert some subjects data
</commit_message>
<xml_diff>
--- a/demos/brainflow_demos/AnalysisAnswer.xlsx
+++ b/demos/brainflow_demos/AnalysisAnswer.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -643,10 +643,10 @@
         <v>0.25</v>
       </c>
       <c r="D10" t="n">
-        <v>0.8266666666666665</v>
+        <v>0.826666666666667</v>
       </c>
       <c r="E10" t="n">
-        <v>123.9204265449724</v>
+        <v>123.920426544972</v>
       </c>
     </row>
     <row r="11">
@@ -664,10 +664,10 @@
         <v>0.5</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9022222222222223</v>
+        <v>0.902222222222222</v>
       </c>
       <c r="E11" t="n">
-        <v>122.9081768002538</v>
+        <v>122.908176800254</v>
       </c>
     </row>
     <row r="12">
@@ -685,10 +685,10 @@
         <v>0.75</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9511111111111111</v>
+        <v>0.951111111111111</v>
       </c>
       <c r="E12" t="n">
-        <v>117.9118315794751</v>
+        <v>117.911831579475</v>
       </c>
     </row>
     <row r="13">
@@ -706,10 +706,2278 @@
         <v>1</v>
       </c>
       <c r="D13" t="n">
-        <v>0.9488888888888889</v>
+        <v>0.948888888888889</v>
       </c>
       <c r="E13" t="n">
-        <v>102.6358259077402</v>
+        <v>102.63582590774</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>jhz</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ssvep-vr-</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.824444444444444</v>
+      </c>
+      <c r="E14" t="n">
+        <v>123.275097276365</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>jhz</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ssvep-vr-</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.937777777777778</v>
+      </c>
+      <c r="E15" t="n">
+        <v>133.351385743164</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>jhz</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ssvep-vr-</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.955555555555555</v>
+      </c>
+      <c r="E16" t="n">
+        <v>119.155323486189</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>jhz</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ssvep-vr-</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.966666666666667</v>
+      </c>
+      <c r="E17" t="n">
+        <v>107.074093936642</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>jhz</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>ssvep-cs-middle-</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.906666666666667</v>
+      </c>
+      <c r="E18" t="n">
+        <v>148.993834296621</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>jhz</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>ssvep-cs-middle-</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.997333333333333</v>
+      </c>
+      <c r="E19" t="n">
+        <v>154.803744203776</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>jhz</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>ssvep-cs-middle-</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" t="n">
+        <v>133.950534706578</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>jhz</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>ssvep-cs-middle-</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" t="n">
+        <v>117.206717868256</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>jhz</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>ssvep-vr-middle-</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.965333333333333</v>
+      </c>
+      <c r="E22" t="n">
+        <v>170.765855015384</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>jhz</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>ssvep-vr-middle-</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.997333333333333</v>
+      </c>
+      <c r="E23" t="n">
+        <v>154.803744203776</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>jhz</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>ssvep-vr-middle-</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" t="n">
+        <v>133.950534706578</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>jhz</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>ssvep-vr-middle-</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.994666666666667</v>
+      </c>
+      <c r="E25" t="n">
+        <v>115.159207035645</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>tll</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>cvep-cs-</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.986666666666667</v>
+      </c>
+      <c r="E26" t="n">
+        <v>180.190455691477</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>tll</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>cvep-cs-</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.995555555555556</v>
+      </c>
+      <c r="E27" t="n">
+        <v>153.953735752343</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>tll</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>cvep-cs-</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.995555555555556</v>
+      </c>
+      <c r="E28" t="n">
+        <v>131.96034493058</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>tll</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>cvep-cs-</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.997777777777778</v>
+      </c>
+      <c r="E29" t="n">
+        <v>116.269236070192</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>tll</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>cvep-vr-</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E30" t="n">
+        <v>116.327592782862</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>tll</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>cvep-vr-</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.811111111111111</v>
+      </c>
+      <c r="E31" t="n">
+        <v>99.5432899376061</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>tll</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>cvep-vr-</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.791111111111111</v>
+      </c>
+      <c r="E32" t="n">
+        <v>81.3333579264371</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>tll</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>cvep-vr-</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.813333333333333</v>
+      </c>
+      <c r="E33" t="n">
+        <v>75.0521481899135</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>tll</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>ssvep-cs-</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="E34" t="n">
+        <v>160.848210294268</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>tll</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>ssvep-cs-</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.997777777777778</v>
+      </c>
+      <c r="E35" t="n">
+        <v>155.02564809359</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>tll</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>ssvep-cs-</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" t="n">
+        <v>133.950534706578</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>tll</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>ssvep-cs-</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1</v>
+      </c>
+      <c r="E37" t="n">
+        <v>117.206717868256</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>tll</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>ssvep-vr-</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="E38" t="n">
+        <v>105.508086476648</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>tll</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>ssvep-vr-</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.815555555555555</v>
+      </c>
+      <c r="E39" t="n">
+        <v>100.59764898139</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>tll</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>ssvep-vr-</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.804444444444444</v>
+      </c>
+      <c r="E40" t="n">
+        <v>83.9791384685181</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>tll</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>ssvep-vr-</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.811111111111111</v>
+      </c>
+      <c r="E41" t="n">
+        <v>74.6574674532046</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>tll</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>ssvep-cs-middle-</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.989333333333333</v>
+      </c>
+      <c r="E42" t="n">
+        <v>181.492694255688</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>tll</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>ssvep-cs-middle-</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.989333333333333</v>
+      </c>
+      <c r="E43" t="n">
+        <v>151.24391187974</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>tll</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>ssvep-cs-middle-</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.994666666666667</v>
+      </c>
+      <c r="E44" t="n">
+        <v>131.610522326452</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>tll</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>ssvep-cs-middle-</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>1</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.994666666666667</v>
+      </c>
+      <c r="E45" t="n">
+        <v>115.159207035645</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>tll</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>ssvep-vr-middle-</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.544</v>
+      </c>
+      <c r="E46" t="n">
+        <v>56.4638447321986</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>tll</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>ssvep-vr-middle-</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="E47" t="n">
+        <v>71.3662225130237</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>tll</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>ssvep-vr-middle-</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0.717333333333333</v>
+      </c>
+      <c r="E48" t="n">
+        <v>67.5983772167134</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>tll</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>ssvep-vr-middle-</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>1</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0.709333333333333</v>
+      </c>
+      <c r="E49" t="n">
+        <v>57.9191569259361</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>stn</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>cvep-cs-</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0.868888888888889</v>
+      </c>
+      <c r="E50" t="n">
+        <v>136.666872238324</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>stn</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>cvep-cs-</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="E51" t="n">
+        <v>147.572118185022</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>stn</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>cvep-cs-</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.982222222222222</v>
+      </c>
+      <c r="E52" t="n">
+        <v>127.214729436245</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>stn</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>cvep-cs-</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>1</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.9911111111111111</v>
+      </c>
+      <c r="E53" t="n">
+        <v>113.991411176826</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>stn</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>cvep-vr-</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.655555555555556</v>
+      </c>
+      <c r="E54" t="n">
+        <v>79.99007887234769</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>stn</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>cvep-vr-</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0.884444444444444</v>
+      </c>
+      <c r="E55" t="n">
+        <v>118.019221364345</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>stn</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>cvep-vr-</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0.933333333333333</v>
+      </c>
+      <c r="E56" t="n">
+        <v>113.132831969712</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>stn</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>cvep-vr-</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>1</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.942222222222222</v>
+      </c>
+      <c r="E57" t="n">
+        <v>101.050513960609</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>stn</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>ssvep-cs-</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0.528888888888889</v>
+      </c>
+      <c r="E58" t="n">
+        <v>53.5494136036953</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>stn</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>ssvep-cs-</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.811111111111111</v>
+      </c>
+      <c r="E59" t="n">
+        <v>99.5432899376061</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>stn</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>ssvep-cs-</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0.888888888888889</v>
+      </c>
+      <c r="E60" t="n">
+        <v>102.19175400167</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>stn</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>ssvep-cs-</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0.926666666666667</v>
+      </c>
+      <c r="E61" t="n">
+        <v>97.4832877075679</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>stn</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>ssvep-vr-</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0.648888888888889</v>
+      </c>
+      <c r="E62" t="n">
+        <v>78.4814169275747</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>stn</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>ssvep-vr-</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0.895555555555556</v>
+      </c>
+      <c r="E63" t="n">
+        <v>121.052226325785</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>stn</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>ssvep-vr-</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0.9577777777777779</v>
+      </c>
+      <c r="E64" t="n">
+        <v>119.785569575612</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>stn</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>ssvep-vr-</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>1</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0.971111111111111</v>
+      </c>
+      <c r="E65" t="n">
+        <v>108.243348833134</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>stn</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>ssvep-cs-middle-</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0.968</v>
+      </c>
+      <c r="E66" t="n">
+        <v>171.875067221875</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>stn</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>ssvep-cs-middle-</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0.994666666666667</v>
+      </c>
+      <c r="E67" t="n">
+        <v>153.54560938086</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>stn</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>ssvep-cs-middle-</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0.994666666666667</v>
+      </c>
+      <c r="E68" t="n">
+        <v>131.610522326452</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>stn</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>ssvep-cs-middle-</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>1</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0.994666666666667</v>
+      </c>
+      <c r="E69" t="n">
+        <v>115.159207035645</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>stn</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>ssvep-vr-middle-</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0.765333333333333</v>
+      </c>
+      <c r="E70" t="n">
+        <v>106.913915659445</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>stn</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>ssvep-vr-middle-</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0.938666666666667</v>
+      </c>
+      <c r="E71" t="n">
+        <v>133.626306173525</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>stn</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>ssvep-vr-middle-</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0.962666666666667</v>
+      </c>
+      <c r="E72" t="n">
+        <v>121.193837123725</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>stn</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>ssvep-vr-middle-</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>1</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0.9733333333333331</v>
+      </c>
+      <c r="E73" t="n">
+        <v>108.83915033503</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>lc</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>cvep-cs-</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0.9555555555555555</v>
+      </c>
+      <c r="E74" t="n">
+        <v>166.8174528806645</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>lc</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>cvep-cs-</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0.9755555555555556</v>
+      </c>
+      <c r="E75" t="n">
+        <v>145.9242609337392</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>lc</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>cvep-cs-</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0.9822222222222223</v>
+      </c>
+      <c r="E76" t="n">
+        <v>127.2147294362453</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>lc</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>cvep-cs-</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>1</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0.9822222222222223</v>
+      </c>
+      <c r="E77" t="n">
+        <v>111.3128882567146</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>lc</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>cvep-vr-</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0.8933333333333333</v>
+      </c>
+      <c r="E78" t="n">
+        <v>144.527698731301</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>lc</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>cvep-vr-</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0.9422222222222223</v>
+      </c>
+      <c r="E79" t="n">
+        <v>134.7340186141453</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>lc</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>cvep-vr-</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0.9511111111111111</v>
+      </c>
+      <c r="E80" t="n">
+        <v>117.9118315794751</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>lc</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>cvep-vr-</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>1</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="E81" t="n">
+        <v>105.369126289314</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>lc</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>ssvep-cs-</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D82" t="n">
+        <v>0.5599999999999999</v>
+      </c>
+      <c r="E82" t="n">
+        <v>59.61921161669361</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>lc</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>ssvep-cs-</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D83" t="n">
+        <v>0.8222222222222222</v>
+      </c>
+      <c r="E83" t="n">
+        <v>102.1934423283185</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>lc</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>ssvep-cs-</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D84" t="n">
+        <v>0.888888888888889</v>
+      </c>
+      <c r="E84" t="n">
+        <v>102.1917540016696</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>lc</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>ssvep-cs-</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>1</v>
+      </c>
+      <c r="D85" t="n">
+        <v>0.9466666666666667</v>
+      </c>
+      <c r="E85" t="n">
+        <v>102.1032074720199</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>lc</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>ssvep-vr-</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D86" t="n">
+        <v>0.6688888888888889</v>
+      </c>
+      <c r="E86" t="n">
+        <v>83.04842462326572</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>lc</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>ssvep-vr-</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D87" t="n">
+        <v>0.8444444444444444</v>
+      </c>
+      <c r="E87" t="n">
+        <v>107.6426070919149</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>lc</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>ssvep-vr-</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0.9111111111111111</v>
+      </c>
+      <c r="E88" t="n">
+        <v>107.5100190237402</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>lc</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>ssvep-vr-</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>1</v>
+      </c>
+      <c r="D89" t="n">
+        <v>0.9266666666666665</v>
+      </c>
+      <c r="E89" t="n">
+        <v>97.48328770756794</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>lc</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>ssvep-cs-middle-</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D90" t="n">
+        <v>0.976</v>
+      </c>
+      <c r="E90" t="n">
+        <v>175.3040896461952</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>lc</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>ssvep-cs-middle-</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D91" t="n">
+        <v>0.976</v>
+      </c>
+      <c r="E91" t="n">
+        <v>146.0867413718293</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>lc</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>ssvep-cs-middle-</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0.968</v>
+      </c>
+      <c r="E92" t="n">
+        <v>122.7679051584821</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>lc</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>ssvep-cs-middle-</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>1</v>
+      </c>
+      <c r="D93" t="n">
+        <v>0.9573333333333334</v>
+      </c>
+      <c r="E93" t="n">
+        <v>104.7016657779226</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>lc</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>ssvep-vr-middle-</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D94" t="n">
+        <v>0.6853333333333333</v>
+      </c>
+      <c r="E94" t="n">
+        <v>86.89707993589823</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>lc</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>ssvep-vr-middle-</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D95" t="n">
+        <v>0.7973333333333334</v>
+      </c>
+      <c r="E95" t="n">
+        <v>96.32148761227164</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>lc</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>ssvep-vr-middle-</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D96" t="n">
+        <v>0.8133333333333332</v>
+      </c>
+      <c r="E96" t="n">
+        <v>85.77388364561547</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>lc</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>ssvep-vr-middle-</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>1</v>
+      </c>
+      <c r="D97" t="n">
+        <v>0.8026666666666668</v>
+      </c>
+      <c r="E97" t="n">
+        <v>73.17029890907426</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>ymm</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>cvep-cs-</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D98" t="n">
+        <v>0.9888888888888889</v>
+      </c>
+      <c r="E98" t="n">
+        <v>181.2726908634922</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>ymm</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>cvep-cs-</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D99" t="n">
+        <v>0.9888888888888889</v>
+      </c>
+      <c r="E99" t="n">
+        <v>151.0605757195768</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>ymm</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>cvep-cs-</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D100" t="n">
+        <v>0.9888888888888889</v>
+      </c>
+      <c r="E100" t="n">
+        <v>129.480493473923</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>ymm</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>cvep-cs-</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>1</v>
+      </c>
+      <c r="D101" t="n">
+        <v>0.9844444444444445</v>
+      </c>
+      <c r="E101" t="n">
+        <v>111.9589594404027</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>ymm</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>cvep-vr-</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D102" t="n">
+        <v>0.7511111111111111</v>
+      </c>
+      <c r="E102" t="n">
+        <v>103.1889580202181</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>ymm</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>cvep-vr-</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D103" t="n">
+        <v>0.8777777777777779</v>
+      </c>
+      <c r="E103" t="n">
+        <v>116.2332878682061</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>ymm</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>cvep-vr-</t>
+        </is>
+      </c>
+      <c r="C104" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D104" t="n">
+        <v>0.928888888888889</v>
+      </c>
+      <c r="E104" t="n">
+        <v>111.9801898422958</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>ymm</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>cvep-vr-</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>1</v>
+      </c>
+      <c r="D105" t="n">
+        <v>0.9533333333333334</v>
+      </c>
+      <c r="E105" t="n">
+        <v>103.7144773852411</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>ymm</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>ssvep-cs-</t>
+        </is>
+      </c>
+      <c r="C106" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D106" t="n">
+        <v>0.9688888888888888</v>
+      </c>
+      <c r="E106" t="n">
+        <v>172.2482770750833</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>ymm</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>ssvep-cs-</t>
+        </is>
+      </c>
+      <c r="C107" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D107" t="n">
+        <v>0.9888888888888889</v>
+      </c>
+      <c r="E107" t="n">
+        <v>151.0605757195768</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>ymm</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>ssvep-cs-</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D108" t="n">
+        <v>0.9911111111111112</v>
+      </c>
+      <c r="E108" t="n">
+        <v>130.2758984878013</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>ymm</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>ssvep-cs-</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>1</v>
+      </c>
+      <c r="D109" t="n">
+        <v>0.9911111111111112</v>
+      </c>
+      <c r="E109" t="n">
+        <v>113.9914111768262</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>ymm</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>ssvep-vr-</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D110" t="n">
+        <v>0.6314814814814815</v>
+      </c>
+      <c r="E110" t="n">
+        <v>74.60553715707708</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>ymm</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>ssvep-vr-</t>
+        </is>
+      </c>
+      <c r="C111" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D111" t="n">
+        <v>0.7685185185185185</v>
+      </c>
+      <c r="E111" t="n">
+        <v>89.79894021732896</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>ymm</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>ssvep-vr-</t>
+        </is>
+      </c>
+      <c r="C112" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D112" t="n">
+        <v>0.8148148148148149</v>
+      </c>
+      <c r="E112" t="n">
+        <v>86.075485710712</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>ymm</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>ssvep-vr-</t>
+        </is>
+      </c>
+      <c r="C113" t="n">
+        <v>1</v>
+      </c>
+      <c r="D113" t="n">
+        <v>0.8314814814814815</v>
+      </c>
+      <c r="E113" t="n">
+        <v>78.32928764282032</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>ymm</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>ssvep-cs-middle-</t>
+        </is>
+      </c>
+      <c r="C114" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D114" t="n">
+        <v>0.9733333333333334</v>
+      </c>
+      <c r="E114" t="n">
+        <v>174.1426405360473</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>ymm</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>ssvep-cs-middle-</t>
+        </is>
+      </c>
+      <c r="C115" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D115" t="n">
+        <v>0.9946666666666667</v>
+      </c>
+      <c r="E115" t="n">
+        <v>153.5456093808605</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>ymm</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>ssvep-cs-middle-</t>
+        </is>
+      </c>
+      <c r="C116" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D116" t="n">
+        <v>0.9973333333333333</v>
+      </c>
+      <c r="E116" t="n">
+        <v>132.6889236032362</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>ymm</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>ssvep-cs-middle-</t>
+        </is>
+      </c>
+      <c r="C117" t="n">
+        <v>1</v>
+      </c>
+      <c r="D117" t="n">
+        <v>0.9973333333333333</v>
+      </c>
+      <c r="E117" t="n">
+        <v>116.1028081528317</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>ymm</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>ssvep-vr-middle-</t>
+        </is>
+      </c>
+      <c r="C118" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D118" t="n">
+        <v>0.5066666666666666</v>
+      </c>
+      <c r="E118" t="n">
+        <v>49.37873971612407</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>ymm</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>ssvep-vr-middle-</t>
+        </is>
+      </c>
+      <c r="C119" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D119" t="n">
+        <v>0.8026666666666668</v>
+      </c>
+      <c r="E119" t="n">
+        <v>97.56039854543235</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>ymm</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>ssvep-vr-middle-</t>
+        </is>
+      </c>
+      <c r="C120" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D120" t="n">
+        <v>0.8800000000000001</v>
+      </c>
+      <c r="E120" t="n">
+        <v>100.1364733602597</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>ymm</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>ssvep-vr-middle-</t>
+        </is>
+      </c>
+      <c r="C121" t="n">
+        <v>1</v>
+      </c>
+      <c r="D121" t="n">
+        <v>0.8959999999999999</v>
+      </c>
+      <c r="E121" t="n">
+        <v>90.88131419708181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>